<commit_message>
Added return of optimal team choices
</commit_message>
<xml_diff>
--- a/vegasodds.xlsx
+++ b/vegasodds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daviddevito/Dropbox/NFL_Survivor_Pool_Algo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF820D4-ADB5-9146-B4BA-5CFB31ECD0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0655A11-B6F7-4748-83C7-D3F09A66F5B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15200" yWindow="740" windowWidth="13620" windowHeight="16780" xr2:uid="{DEA9C9A6-06A7-BE49-B21F-182B08E4DAEE}"/>
+    <workbookView xWindow="13860" yWindow="740" windowWidth="15320" windowHeight="16780" xr2:uid="{DEA9C9A6-06A7-BE49-B21F-182B08E4DAEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Week1</t>
   </si>
@@ -183,9 +183,6 @@
   </si>
   <si>
     <t>Week17</t>
-  </si>
-  <si>
-    <t>Week18</t>
   </si>
 </sst>
 </file>
@@ -201,12 +198,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -221,8 +224,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,8 +563,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D62FC5C-F8D9-694E-BAE3-7B86A4BA66FF}">
   <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -569,67 +574,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="S1" t="s">
-        <v>49</v>
-      </c>
+      <c r="S1" s="1"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2">
-        <v>-3.5</v>
+        <v>-4.5</v>
       </c>
       <c r="C2">
         <v>-6.5</v>
@@ -640,47 +643,44 @@
       <c r="E2">
         <v>-12</v>
       </c>
-      <c r="F2">
-        <v>-3.5</v>
+      <c r="F2" s="1">
+        <v>-9.5</v>
       </c>
       <c r="G2">
+        <v>-5</v>
+      </c>
+      <c r="H2">
+        <v>-1</v>
+      </c>
+      <c r="I2">
+        <v>-5.5</v>
+      </c>
+      <c r="J2">
+        <v>1000</v>
+      </c>
+      <c r="K2">
+        <v>-7</v>
+      </c>
+      <c r="L2">
+        <v>-9</v>
+      </c>
+      <c r="M2">
+        <v>-2.5</v>
+      </c>
+      <c r="N2">
+        <v>-2</v>
+      </c>
+      <c r="O2">
+        <v>-5.5</v>
+      </c>
+      <c r="P2">
         <v>-6.5</v>
       </c>
-      <c r="H2">
-        <v>-3.5</v>
-      </c>
-      <c r="I2">
-        <v>-6.5</v>
-      </c>
-      <c r="J2">
-        <v>-4</v>
-      </c>
-      <c r="K2">
-        <v>-12</v>
-      </c>
-      <c r="L2">
-        <v>-3.5</v>
-      </c>
-      <c r="M2">
-        <v>-6.5</v>
-      </c>
-      <c r="N2">
-        <v>-3.5</v>
-      </c>
-      <c r="O2">
-        <v>-6.5</v>
-      </c>
-      <c r="P2">
-        <v>-4</v>
-      </c>
       <c r="Q2">
-        <v>-12</v>
+        <v>-1</v>
       </c>
       <c r="R2">
-        <v>-3.5</v>
-      </c>
-      <c r="S2">
-        <v>-6.5</v>
+        <v>-4.5</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
@@ -688,7 +688,7 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-4.5</v>
+        <v>-4</v>
       </c>
       <c r="C3">
         <v>3.5</v>
@@ -700,46 +700,43 @@
         <v>-1</v>
       </c>
       <c r="F3">
-        <v>-4.5</v>
+        <v>-5.5</v>
       </c>
       <c r="G3">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>-4.5</v>
+        <v>1000</v>
       </c>
       <c r="I3">
-        <v>3.5</v>
+        <v>-2</v>
       </c>
       <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>-1</v>
+        <v>-1.5</v>
+      </c>
+      <c r="K3" s="1">
+        <v>-5.5</v>
       </c>
       <c r="L3">
-        <v>-4.5</v>
+        <v>-1</v>
       </c>
       <c r="M3">
-        <v>3.5</v>
+        <v>-3</v>
       </c>
       <c r="N3">
-        <v>-4.5</v>
+        <v>4</v>
       </c>
       <c r="O3">
-        <v>3.5</v>
+        <v>5.5</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Q3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="R3">
-        <v>-4.5</v>
-      </c>
-      <c r="S3">
-        <v>3.5</v>
+        <v>-3.5</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -752,61 +749,58 @@
       <c r="C4">
         <v>3.5</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>-6.5</v>
       </c>
       <c r="E4">
         <v>-5.5</v>
       </c>
       <c r="F4">
-        <v>-8.5</v>
+        <v>-1.5</v>
       </c>
       <c r="G4">
-        <v>3.5</v>
+        <v>-4.5</v>
       </c>
       <c r="H4">
-        <v>-8.5</v>
+        <v>-1</v>
       </c>
       <c r="I4">
-        <v>3.5</v>
+        <v>-3</v>
       </c>
       <c r="J4">
-        <v>-6.5</v>
+        <v>-7</v>
       </c>
       <c r="K4">
-        <v>-5.5</v>
+        <v>3</v>
       </c>
       <c r="L4">
-        <v>-8.5</v>
+        <v>-2</v>
       </c>
       <c r="M4">
-        <v>3.5</v>
+        <v>1000</v>
       </c>
       <c r="N4">
-        <v>-8.5</v>
+        <v>-5</v>
       </c>
       <c r="O4">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="P4">
-        <v>-6.5</v>
+        <v>-4.5</v>
       </c>
       <c r="Q4">
-        <v>-5.5</v>
+        <v>-3.5</v>
       </c>
       <c r="R4">
-        <v>-8.5</v>
-      </c>
-      <c r="S4">
-        <v>3.5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
-        <v>-6</v>
+      <c r="B5" s="1">
+        <v>-6.5</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -818,46 +812,43 @@
         <v>3</v>
       </c>
       <c r="F5">
-        <v>-6</v>
+        <v>1.5</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H5">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="J5">
-        <v>-3.5</v>
+        <v>-3</v>
       </c>
       <c r="K5">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="L5">
-        <v>-6</v>
+        <v>-1</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="N5">
-        <v>-6</v>
+        <v>2</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="P5">
-        <v>-3.5</v>
+        <v>2</v>
       </c>
       <c r="Q5">
-        <v>3</v>
+        <v>-8.5</v>
       </c>
       <c r="R5">
-        <v>-6</v>
-      </c>
-      <c r="S5">
-        <v>1</v>
+        <v>-2.5</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
@@ -865,7 +856,7 @@
         <v>26</v>
       </c>
       <c r="B6">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -877,46 +868,43 @@
         <v>7</v>
       </c>
       <c r="F6">
-        <v>5.5</v>
+        <v>-1</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="H6">
-        <v>5.5</v>
+        <v>3.5</v>
       </c>
       <c r="I6">
-        <v>3</v>
+        <v>-2.5</v>
       </c>
       <c r="J6">
+        <v>10.5</v>
+      </c>
+      <c r="K6">
+        <v>9</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="M6">
+        <v>3</v>
+      </c>
+      <c r="N6">
         <v>3.5</v>
       </c>
-      <c r="K6">
-        <v>7</v>
-      </c>
-      <c r="L6">
-        <v>5.5</v>
-      </c>
-      <c r="M6">
-        <v>3</v>
-      </c>
-      <c r="N6">
-        <v>5.5</v>
-      </c>
       <c r="O6">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="P6">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="Q6">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="R6">
-        <v>5.5</v>
-      </c>
-      <c r="S6">
-        <v>3</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
@@ -936,46 +924,43 @@
         <v>-1.5</v>
       </c>
       <c r="F7">
-        <v>-2.5</v>
+        <v>-3</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H7">
-        <v>-2.5</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>2</v>
-      </c>
-      <c r="J7">
-        <v>-5.5</v>
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>-3</v>
       </c>
       <c r="K7">
-        <v>-1.5</v>
+        <v>1000</v>
       </c>
       <c r="L7">
-        <v>-2.5</v>
+        <v>-2</v>
       </c>
       <c r="M7">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="N7">
-        <v>-2.5</v>
+        <v>-3.5</v>
       </c>
       <c r="O7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P7">
-        <v>-5.5</v>
+        <v>3</v>
       </c>
       <c r="Q7">
-        <v>-1.5</v>
+        <v>3.5</v>
       </c>
       <c r="R7">
-        <v>-2.5</v>
-      </c>
-      <c r="S7">
-        <v>2</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
@@ -995,46 +980,43 @@
         <v>3</v>
       </c>
       <c r="F8">
-        <v>-3.5</v>
+        <v>3</v>
       </c>
       <c r="G8">
-        <v>6.5</v>
+        <v>1.5</v>
       </c>
       <c r="H8">
-        <v>-3.5</v>
+        <v>5</v>
       </c>
       <c r="I8">
-        <v>6.5</v>
+        <v>-1</v>
       </c>
       <c r="J8">
-        <v>-3.5</v>
+        <v>7</v>
       </c>
       <c r="K8">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="L8">
-        <v>-3.5</v>
+        <v>1000</v>
       </c>
       <c r="M8">
-        <v>6.5</v>
+        <v>-1</v>
       </c>
       <c r="N8">
-        <v>-3.5</v>
-      </c>
-      <c r="O8">
-        <v>6.5</v>
+        <v>-2</v>
+      </c>
+      <c r="O8" s="1">
+        <v>-2.5</v>
       </c>
       <c r="P8">
-        <v>-3.5</v>
+        <v>3</v>
       </c>
       <c r="Q8">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="R8">
-        <v>-3.5</v>
-      </c>
-      <c r="S8">
-        <v>6.5</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
@@ -1042,7 +1024,7 @@
         <v>21</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="C9">
         <v>2.5</v>
@@ -1054,46 +1036,43 @@
         <v>-3</v>
       </c>
       <c r="F9">
+        <v>9.5</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>-1</v>
+      </c>
+      <c r="I9">
         <v>6</v>
       </c>
-      <c r="G9">
-        <v>2.5</v>
-      </c>
-      <c r="H9">
-        <v>6</v>
-      </c>
-      <c r="I9">
-        <v>2.5</v>
-      </c>
       <c r="J9">
-        <v>3.5</v>
+        <v>1.5</v>
       </c>
       <c r="K9">
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="L9">
-        <v>6</v>
+        <v>1000</v>
       </c>
       <c r="M9">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="N9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="O9">
-        <v>2.5</v>
-      </c>
-      <c r="P9">
-        <v>3.5</v>
+        <v>-1</v>
+      </c>
+      <c r="P9" s="1">
+        <v>-3.5</v>
       </c>
       <c r="Q9">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="R9">
-        <v>6</v>
-      </c>
-      <c r="S9">
-        <v>2.5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
@@ -1113,46 +1092,43 @@
         <v>3.5</v>
       </c>
       <c r="F10">
-        <v>-3</v>
+        <v>1000</v>
       </c>
       <c r="G10">
-        <v>-3.5</v>
+        <v>-2.5</v>
       </c>
       <c r="H10">
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>-3.5</v>
+        <v>-3</v>
       </c>
       <c r="J10">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="K10">
-        <v>3.5</v>
+        <v>-4</v>
       </c>
       <c r="L10">
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="M10">
-        <v>-3.5</v>
+        <v>3</v>
       </c>
       <c r="N10">
-        <v>-3</v>
+        <v>2.5</v>
       </c>
       <c r="O10">
-        <v>-3.5</v>
+        <v>6.5</v>
       </c>
       <c r="P10">
-        <v>1.5</v>
+        <v>-3</v>
       </c>
       <c r="Q10">
-        <v>3.5</v>
+        <v>-4</v>
       </c>
       <c r="R10">
-        <v>-3</v>
-      </c>
-      <c r="S10">
-        <v>-3.5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
@@ -1172,46 +1148,43 @@
         <v>-3.5</v>
       </c>
       <c r="F11">
-        <v>-3</v>
+        <v>-8</v>
       </c>
       <c r="G11">
-        <v>-3.5</v>
+        <v>1000</v>
       </c>
       <c r="H11">
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>-3.5</v>
+        <v>-5.5</v>
       </c>
       <c r="J11">
-        <v>-3.5</v>
+        <v>-7</v>
       </c>
       <c r="K11">
-        <v>-3.5</v>
+        <v>-9</v>
       </c>
       <c r="L11">
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="M11">
-        <v>-3.5</v>
+        <v>-7</v>
       </c>
       <c r="N11">
-        <v>-3</v>
+        <v>-7.5</v>
       </c>
       <c r="O11">
-        <v>-3.5</v>
+        <v>-6.5</v>
       </c>
       <c r="P11">
-        <v>-3.5</v>
+        <v>-3</v>
       </c>
       <c r="Q11">
-        <v>-3.5</v>
-      </c>
-      <c r="R11">
-        <v>-3</v>
-      </c>
-      <c r="S11">
-        <v>-3.5</v>
+        <v>-4.5</v>
+      </c>
+      <c r="R11" s="1">
+        <v>-4</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
@@ -1219,7 +1192,7 @@
         <v>23</v>
       </c>
       <c r="B12">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <v>4.5</v>
@@ -1234,43 +1207,40 @@
         <v>2.5</v>
       </c>
       <c r="G12">
-        <v>4.5</v>
+        <v>-1.5</v>
       </c>
       <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>4</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>2</v>
+      </c>
+      <c r="L12">
+        <v>4</v>
+      </c>
+      <c r="M12">
         <v>2.5</v>
       </c>
-      <c r="I12">
-        <v>4.5</v>
-      </c>
-      <c r="J12">
-        <v>-1</v>
-      </c>
-      <c r="K12">
-        <v>-1</v>
-      </c>
-      <c r="L12">
-        <v>2.5</v>
-      </c>
-      <c r="M12">
-        <v>4.5</v>
-      </c>
       <c r="N12">
-        <v>2.5</v>
+        <v>-2.5</v>
       </c>
       <c r="O12">
-        <v>4.5</v>
+        <v>1000</v>
       </c>
       <c r="P12">
-        <v>-1</v>
+        <v>-2.5</v>
       </c>
       <c r="Q12">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="R12">
-        <v>2.5</v>
-      </c>
-      <c r="S12">
-        <v>4.5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
@@ -1290,46 +1260,43 @@
         <v>3</v>
       </c>
       <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>8.5</v>
+      </c>
+      <c r="H13">
+        <v>-3</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>1.5</v>
+      </c>
+      <c r="K13">
+        <v>1.5</v>
+      </c>
+      <c r="L13">
+        <v>7</v>
+      </c>
+      <c r="M13">
         <v>3.5</v>
       </c>
-      <c r="G13">
-        <v>-2.5</v>
-      </c>
-      <c r="H13">
-        <v>3.5</v>
-      </c>
-      <c r="I13">
-        <v>-2.5</v>
-      </c>
-      <c r="J13">
-        <v>6.5</v>
-      </c>
-      <c r="K13">
-        <v>3</v>
-      </c>
-      <c r="L13">
-        <v>3.5</v>
-      </c>
-      <c r="M13">
-        <v>-2.5</v>
-      </c>
       <c r="N13">
-        <v>3.5</v>
+        <v>-1.5</v>
       </c>
       <c r="O13">
-        <v>-2.5</v>
+        <v>1000</v>
       </c>
       <c r="P13">
-        <v>6.5</v>
+        <v>3</v>
       </c>
       <c r="Q13">
         <v>3</v>
       </c>
       <c r="R13">
-        <v>3.5</v>
-      </c>
-      <c r="S13">
-        <v>-2.5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
@@ -1349,46 +1316,43 @@
         <v>-5</v>
       </c>
       <c r="F14">
-        <v>2.5</v>
+        <v>-1.5</v>
       </c>
       <c r="G14">
+        <v>-1</v>
+      </c>
+      <c r="H14">
+        <v>1000</v>
+      </c>
+      <c r="I14">
+        <v>5.5</v>
+      </c>
+      <c r="J14">
+        <v>-1</v>
+      </c>
+      <c r="K14">
+        <v>-2</v>
+      </c>
+      <c r="L14">
+        <v>-3</v>
+      </c>
+      <c r="M14">
+        <v>-3.5</v>
+      </c>
+      <c r="N14" s="1">
+        <v>-8</v>
+      </c>
+      <c r="O14">
+        <v>-1</v>
+      </c>
+      <c r="P14">
         <v>-6.5</v>
       </c>
-      <c r="H14">
-        <v>2.5</v>
-      </c>
-      <c r="I14">
-        <v>-6.5</v>
-      </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-      <c r="K14">
-        <v>-5</v>
-      </c>
-      <c r="L14">
-        <v>2.5</v>
-      </c>
-      <c r="M14">
-        <v>-6.5</v>
-      </c>
-      <c r="N14">
-        <v>2.5</v>
-      </c>
-      <c r="O14">
-        <v>-6.5</v>
-      </c>
-      <c r="P14">
-        <v>1</v>
-      </c>
       <c r="Q14">
-        <v>-5</v>
+        <v>-4.5</v>
       </c>
       <c r="R14">
         <v>2.5</v>
-      </c>
-      <c r="S14">
-        <v>-6.5</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
@@ -1408,46 +1372,43 @@
         <v>-6.5</v>
       </c>
       <c r="F15">
-        <v>-3</v>
+        <v>-4.5</v>
       </c>
       <c r="G15">
-        <v>-1</v>
+        <v>1000</v>
       </c>
       <c r="H15">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="I15">
-        <v>-1</v>
+        <v>-6</v>
       </c>
       <c r="J15">
-        <v>-2.5</v>
+        <v>3</v>
       </c>
       <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
         <v>-6.5</v>
       </c>
-      <c r="L15">
-        <v>-3</v>
-      </c>
-      <c r="M15">
-        <v>-1</v>
+      <c r="M15" s="1">
+        <v>-7.5</v>
       </c>
       <c r="N15">
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="O15">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="P15">
-        <v>-2.5</v>
+        <v>2.5</v>
       </c>
       <c r="Q15">
-        <v>-6.5</v>
+        <v>1</v>
       </c>
       <c r="R15">
-        <v>-3</v>
-      </c>
-      <c r="S15">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
@@ -1455,7 +1416,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>-2.5</v>
+        <v>-2</v>
       </c>
       <c r="C16">
         <v>-3.5</v>
@@ -1467,37 +1428,37 @@
         <v>-3</v>
       </c>
       <c r="F16">
-        <v>-2.5</v>
+        <v>1000</v>
       </c>
       <c r="G16">
-        <v>-3.5</v>
+        <v>-3</v>
       </c>
       <c r="H16">
-        <v>-2.5</v>
+        <v>-4.5</v>
       </c>
       <c r="I16">
-        <v>-3.5</v>
+        <v>3</v>
       </c>
       <c r="J16">
-        <v>-3</v>
+        <v>-3.5</v>
       </c>
       <c r="K16">
-        <v>-3</v>
-      </c>
-      <c r="L16">
-        <v>-2.5</v>
+        <v>2</v>
+      </c>
+      <c r="L16" s="1">
+        <v>-7</v>
       </c>
       <c r="M16">
-        <v>-3.5</v>
+        <v>0.5</v>
       </c>
       <c r="N16">
-        <v>-2.5</v>
+        <v>3.5</v>
       </c>
       <c r="O16">
-        <v>-3.5</v>
+        <v>-7.5</v>
       </c>
       <c r="P16">
-        <v>-3</v>
+        <v>-4.5</v>
       </c>
       <c r="Q16">
         <v>-3</v>
@@ -1505,11 +1466,8 @@
       <c r="R16">
         <v>-2.5</v>
       </c>
-      <c r="S16">
-        <v>-3.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1529,46 +1487,43 @@
         <v>-3</v>
       </c>
       <c r="G17">
-        <v>3.5</v>
+        <v>-3.5</v>
       </c>
       <c r="H17">
-        <v>-3</v>
+        <v>-3.5</v>
       </c>
       <c r="I17">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="J17">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="K17">
-        <v>-3.5</v>
+        <v>-1</v>
       </c>
       <c r="L17">
         <v>-3</v>
       </c>
       <c r="M17">
-        <v>3.5</v>
+        <v>1000</v>
       </c>
       <c r="N17">
-        <v>-3</v>
+        <v>-2.5</v>
       </c>
       <c r="O17">
-        <v>3.5</v>
+        <v>-1</v>
       </c>
       <c r="P17">
-        <v>3.5</v>
+        <v>-1</v>
       </c>
       <c r="Q17">
-        <v>-3.5</v>
+        <v>-4.5</v>
       </c>
       <c r="R17">
-        <v>-3</v>
-      </c>
-      <c r="S17">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1585,49 +1540,46 @@
         <v>5</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>3.5</v>
       </c>
       <c r="G18">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>4.5</v>
       </c>
       <c r="I18">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="J18">
-        <v>5.5</v>
+        <v>-1.5</v>
       </c>
       <c r="K18">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="L18">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="M18">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="N18">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="O18">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="P18">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="Q18">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="R18">
-        <v>1</v>
-      </c>
-      <c r="S18">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1644,56 +1596,53 @@
         <v>3.5</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>-2.5</v>
       </c>
       <c r="G19">
-        <v>-2</v>
-      </c>
-      <c r="H19">
-        <v>3</v>
+        <v>-1</v>
+      </c>
+      <c r="H19" s="1">
+        <v>-6.5</v>
       </c>
       <c r="I19">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="J19">
         <v>3.5</v>
       </c>
       <c r="K19">
-        <v>3.5</v>
+        <v>-3</v>
       </c>
       <c r="L19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M19">
-        <v>-2</v>
+        <v>1000</v>
       </c>
       <c r="N19">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="O19">
-        <v>-2</v>
+        <v>-1.5</v>
       </c>
       <c r="P19">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="Q19">
-        <v>3.5</v>
+        <v>-1</v>
       </c>
       <c r="R19">
-        <v>3</v>
-      </c>
-      <c r="S19">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>33</v>
       </c>
       <c r="B20">
-        <v>3.5</v>
-      </c>
-      <c r="C20">
+        <v>4.5</v>
+      </c>
+      <c r="C20" s="1">
         <v>-4</v>
       </c>
       <c r="D20">
@@ -1703,49 +1652,46 @@
         <v>-7</v>
       </c>
       <c r="F20">
-        <v>3.5</v>
+        <v>-4</v>
       </c>
       <c r="G20">
+        <v>-1.5</v>
+      </c>
+      <c r="H20">
+        <v>-1</v>
+      </c>
+      <c r="I20">
+        <v>-4.5</v>
+      </c>
+      <c r="J20">
+        <v>-3</v>
+      </c>
+      <c r="K20">
+        <v>-3</v>
+      </c>
+      <c r="L20">
         <v>-4</v>
       </c>
-      <c r="H20">
-        <v>3.5</v>
-      </c>
-      <c r="I20">
-        <v>-4</v>
-      </c>
-      <c r="J20">
-        <v>-7</v>
-      </c>
-      <c r="K20">
-        <v>-7</v>
-      </c>
-      <c r="L20">
-        <v>3.5</v>
-      </c>
       <c r="M20">
-        <v>-4</v>
+        <v>1000</v>
       </c>
       <c r="N20">
-        <v>3.5</v>
+        <v>-4.5</v>
       </c>
       <c r="O20">
-        <v>-4</v>
+        <v>2</v>
       </c>
       <c r="P20">
-        <v>-7</v>
+        <v>-1</v>
       </c>
       <c r="Q20">
-        <v>-7</v>
+        <v>-3</v>
       </c>
       <c r="R20">
-        <v>3.5</v>
-      </c>
-      <c r="S20">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1758,58 +1704,55 @@
       <c r="D21">
         <v>-3.5</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <v>-6</v>
       </c>
       <c r="F21">
-        <v>-3.5</v>
+        <v>1000</v>
       </c>
       <c r="G21">
-        <v>-6.5</v>
+        <v>1</v>
       </c>
       <c r="H21">
-        <v>-3.5</v>
+        <v>-3</v>
       </c>
       <c r="I21">
-        <v>-6.5</v>
+        <v>-7.5</v>
       </c>
       <c r="J21">
-        <v>-3.5</v>
+        <v>1.5</v>
       </c>
       <c r="K21">
-        <v>-6</v>
+        <v>1</v>
       </c>
       <c r="L21">
-        <v>-3.5</v>
+        <v>-4</v>
       </c>
       <c r="M21">
-        <v>-6.5</v>
+        <v>-2.5</v>
       </c>
       <c r="N21">
-        <v>-3.5</v>
+        <v>-4</v>
       </c>
       <c r="O21">
-        <v>-6.5</v>
+        <v>-2.5</v>
       </c>
       <c r="P21">
-        <v>-3.5</v>
+        <v>-2</v>
       </c>
       <c r="Q21">
-        <v>-6</v>
+        <v>-1</v>
       </c>
       <c r="R21">
-        <v>-3.5</v>
-      </c>
-      <c r="S21">
-        <v>-6.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>15</v>
       </c>
       <c r="B22">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="C22">
         <v>-4.5</v>
@@ -1821,49 +1764,46 @@
         <v>-5.5</v>
       </c>
       <c r="F22">
+        <v>1.5</v>
+      </c>
+      <c r="G22">
+        <v>-5</v>
+      </c>
+      <c r="H22">
+        <v>-2.5</v>
+      </c>
+      <c r="I22">
+        <v>-1</v>
+      </c>
+      <c r="J22">
+        <v>-1.5</v>
+      </c>
+      <c r="K22">
+        <v>1000</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
         <v>2.5</v>
       </c>
-      <c r="G22">
-        <v>-4.5</v>
-      </c>
-      <c r="H22">
+      <c r="N22">
+        <v>-3</v>
+      </c>
+      <c r="O22">
         <v>2.5</v>
       </c>
-      <c r="I22">
-        <v>-4.5</v>
-      </c>
-      <c r="J22">
-        <v>-4</v>
-      </c>
-      <c r="K22">
-        <v>-5.5</v>
-      </c>
-      <c r="L22">
-        <v>2.5</v>
-      </c>
-      <c r="M22">
-        <v>-4.5</v>
-      </c>
-      <c r="N22">
-        <v>2.5</v>
-      </c>
-      <c r="O22">
-        <v>-4.5</v>
-      </c>
       <c r="P22">
-        <v>-4</v>
-      </c>
-      <c r="Q22">
-        <v>-5.5</v>
+        <v>-1</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>-5</v>
       </c>
       <c r="R22">
-        <v>2.5</v>
-      </c>
-      <c r="S22">
-        <v>-4.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1880,49 +1820,46 @@
         <v>5.5</v>
       </c>
       <c r="F23">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="G23">
-        <v>-3.5</v>
+        <v>3.5</v>
       </c>
       <c r="H23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I23">
-        <v>-3.5</v>
+        <v>2.5</v>
       </c>
       <c r="J23">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K23">
-        <v>5.5</v>
+        <v>1</v>
       </c>
       <c r="L23">
-        <v>4</v>
+        <v>1000</v>
       </c>
       <c r="M23">
-        <v>-3.5</v>
+        <v>7</v>
       </c>
       <c r="N23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O23">
-        <v>-3.5</v>
+        <v>7.5</v>
       </c>
       <c r="P23">
-        <v>4</v>
+        <v>6.5</v>
       </c>
       <c r="Q23">
-        <v>5.5</v>
+        <v>1</v>
       </c>
       <c r="R23">
-        <v>4</v>
-      </c>
-      <c r="S23">
-        <v>-3.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -1939,49 +1876,46 @@
         <v>12</v>
       </c>
       <c r="F24">
+        <v>4.5</v>
+      </c>
+      <c r="G24">
+        <v>4.5</v>
+      </c>
+      <c r="H24">
+        <v>6.5</v>
+      </c>
+      <c r="I24">
+        <v>4.5</v>
+      </c>
+      <c r="J24">
+        <v>2.5</v>
+      </c>
+      <c r="K24">
+        <v>5.5</v>
+      </c>
+      <c r="L24">
+        <v>4</v>
+      </c>
+      <c r="M24">
+        <v>7.5</v>
+      </c>
+      <c r="N24">
+        <v>2.5</v>
+      </c>
+      <c r="O24">
+        <v>1000</v>
+      </c>
+      <c r="P24">
+        <v>3.5</v>
+      </c>
+      <c r="Q24">
         <v>8.5</v>
       </c>
-      <c r="G24">
-        <v>3</v>
-      </c>
-      <c r="H24">
-        <v>8.5</v>
-      </c>
-      <c r="I24">
-        <v>3</v>
-      </c>
-      <c r="J24">
-        <v>7</v>
-      </c>
-      <c r="K24">
-        <v>12</v>
-      </c>
-      <c r="L24">
-        <v>8.5</v>
-      </c>
-      <c r="M24">
-        <v>3</v>
-      </c>
-      <c r="N24">
-        <v>8.5</v>
-      </c>
-      <c r="O24">
-        <v>3</v>
-      </c>
-      <c r="P24">
-        <v>7</v>
-      </c>
-      <c r="Q24">
-        <v>12</v>
-      </c>
       <c r="R24">
-        <v>8.5</v>
-      </c>
-      <c r="S24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1998,49 +1932,46 @@
         <v>1.5</v>
       </c>
       <c r="F25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>4.5</v>
+      </c>
+      <c r="I25">
+        <v>5.5</v>
+      </c>
+      <c r="J25">
+        <v>7</v>
+      </c>
+      <c r="K25">
+        <v>1000</v>
+      </c>
+      <c r="L25">
+        <v>6.5</v>
+      </c>
+      <c r="M25">
+        <v>-3</v>
+      </c>
+      <c r="N25">
         <v>7.5</v>
       </c>
-      <c r="H25">
-        <v>3</v>
-      </c>
-      <c r="I25">
-        <v>7.5</v>
-      </c>
-      <c r="J25">
-        <v>-4</v>
-      </c>
-      <c r="K25">
-        <v>1.5</v>
-      </c>
-      <c r="L25">
-        <v>3</v>
-      </c>
-      <c r="M25">
-        <v>7.5</v>
-      </c>
-      <c r="N25">
-        <v>3</v>
-      </c>
       <c r="O25">
-        <v>7.5</v>
+        <v>2.5</v>
       </c>
       <c r="P25">
-        <v>-4</v>
+        <v>1</v>
       </c>
       <c r="Q25">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="R25">
-        <v>3</v>
-      </c>
-      <c r="S25">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -2057,49 +1988,46 @@
         <v>1</v>
       </c>
       <c r="F26">
-        <v>3.5</v>
+        <v>-1.5</v>
       </c>
       <c r="G26">
-        <v>-2.5</v>
+        <v>1000</v>
       </c>
       <c r="H26">
-        <v>3.5</v>
+        <v>-4.5</v>
       </c>
       <c r="I26">
-        <v>-2.5</v>
+        <v>-3.5</v>
       </c>
       <c r="J26">
-        <v>4</v>
+        <v>-1.5</v>
       </c>
       <c r="K26">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="L26">
-        <v>3.5</v>
+        <v>-4</v>
       </c>
       <c r="M26">
-        <v>-2.5</v>
+        <v>-0.5</v>
       </c>
       <c r="N26">
-        <v>3.5</v>
+        <v>-1.5</v>
       </c>
       <c r="O26">
-        <v>-2.5</v>
+        <v>1</v>
       </c>
       <c r="P26">
-        <v>4</v>
+        <v>6.5</v>
       </c>
       <c r="Q26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R26">
-        <v>3.5</v>
-      </c>
-      <c r="S26">
-        <v>-2.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -2116,49 +2044,46 @@
         <v>-3</v>
       </c>
       <c r="F27">
-        <v>3</v>
-      </c>
-      <c r="G27">
-        <v>-7.5</v>
+        <v>1.5</v>
+      </c>
+      <c r="G27" s="1">
+        <v>-8.5</v>
       </c>
       <c r="H27">
-        <v>3</v>
+        <v>-5</v>
       </c>
       <c r="I27">
-        <v>-7.5</v>
+        <v>-1</v>
       </c>
       <c r="J27">
-        <v>-1</v>
+        <v>-10.5</v>
       </c>
       <c r="K27">
         <v>-3</v>
       </c>
       <c r="L27">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="M27">
-        <v>-7.5</v>
+        <v>-3</v>
       </c>
       <c r="N27">
-        <v>3</v>
+        <v>-3.5</v>
       </c>
       <c r="O27">
-        <v>-7.5</v>
+        <v>1000</v>
       </c>
       <c r="P27">
-        <v>-1</v>
+        <v>-6.5</v>
       </c>
       <c r="Q27">
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="R27">
-        <v>3</v>
-      </c>
-      <c r="S27">
-        <v>-7.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -2175,54 +2100,51 @@
         <v>3.5</v>
       </c>
       <c r="F28">
-        <v>-4</v>
+        <v>8</v>
       </c>
       <c r="G28">
-        <v>6.5</v>
+        <v>-1.5</v>
       </c>
       <c r="H28">
-        <v>-4</v>
+        <v>-3.5</v>
       </c>
       <c r="I28">
-        <v>6.5</v>
+        <v>3</v>
       </c>
       <c r="J28">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="K28">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="L28">
-        <v>-4</v>
+        <v>2</v>
       </c>
       <c r="M28">
-        <v>6.5</v>
+        <v>1000</v>
       </c>
       <c r="N28">
-        <v>-4</v>
+        <v>1.5</v>
       </c>
       <c r="O28">
-        <v>6.5</v>
+        <v>-1</v>
       </c>
       <c r="P28">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="Q28">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="R28">
-        <v>-4</v>
-      </c>
-      <c r="S28">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29">
-        <v>-5.5</v>
+        <v>-6</v>
       </c>
       <c r="C29">
         <v>-3</v>
@@ -2234,49 +2156,46 @@
         <v>6</v>
       </c>
       <c r="F29">
-        <v>-5.5</v>
+        <v>-3.5</v>
       </c>
       <c r="G29">
-        <v>-3</v>
+        <v>5</v>
       </c>
       <c r="H29">
-        <v>-5.5</v>
+        <v>3.5</v>
       </c>
       <c r="I29">
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="J29">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="K29">
-        <v>6</v>
+        <v>1000</v>
       </c>
       <c r="L29">
-        <v>-5.5</v>
+        <v>9</v>
       </c>
       <c r="M29">
         <v>-3</v>
       </c>
       <c r="N29">
-        <v>-5.5</v>
+        <v>4.5</v>
       </c>
       <c r="O29">
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="P29">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="Q29">
-        <v>6</v>
+        <v>-2</v>
       </c>
       <c r="R29">
-        <v>-5.5</v>
-      </c>
-      <c r="S29">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -2293,54 +2212,51 @@
         <v>1</v>
       </c>
       <c r="F30">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="G30">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="H30">
-        <v>3</v>
-      </c>
-      <c r="I30">
-        <v>-3</v>
+        <v>1</v>
+      </c>
+      <c r="I30" s="1">
+        <v>-4</v>
       </c>
       <c r="J30">
+        <v>1000</v>
+      </c>
+      <c r="K30">
         <v>-1.5</v>
       </c>
-      <c r="K30">
-        <v>1</v>
-      </c>
       <c r="L30">
         <v>3</v>
       </c>
       <c r="M30">
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="N30">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O30">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="P30">
-        <v>-1.5</v>
+        <v>4.5</v>
       </c>
       <c r="Q30">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="R30">
-        <v>3</v>
-      </c>
-      <c r="S30">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>22</v>
       </c>
       <c r="B31">
-        <v>-2.5</v>
+        <v>-3</v>
       </c>
       <c r="C31">
         <v>-3.5</v>
@@ -2352,54 +2268,51 @@
         <v>-3.5</v>
       </c>
       <c r="F31">
+        <v>-1.5</v>
+      </c>
+      <c r="G31">
+        <v>-4.5</v>
+      </c>
+      <c r="H31">
+        <v>2.5</v>
+      </c>
+      <c r="I31">
+        <v>-4</v>
+      </c>
+      <c r="J31">
+        <v>3</v>
+      </c>
+      <c r="K31">
+        <v>-1</v>
+      </c>
+      <c r="L31">
+        <v>3</v>
+      </c>
+      <c r="M31">
+        <v>-6</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <v>1000</v>
+      </c>
+      <c r="P31">
         <v>-2.5</v>
       </c>
-      <c r="G31">
-        <v>-3.5</v>
-      </c>
-      <c r="H31">
-        <v>-2.5</v>
-      </c>
-      <c r="I31">
-        <v>-3.5</v>
-      </c>
-      <c r="J31">
-        <v>-4</v>
-      </c>
-      <c r="K31">
-        <v>-3.5</v>
-      </c>
-      <c r="L31">
-        <v>-2.5</v>
-      </c>
-      <c r="M31">
-        <v>-3.5</v>
-      </c>
-      <c r="N31">
-        <v>-2.5</v>
-      </c>
-      <c r="O31">
-        <v>-3.5</v>
-      </c>
-      <c r="P31">
-        <v>-4</v>
-      </c>
       <c r="Q31">
-        <v>-3.5</v>
+        <v>4.5</v>
       </c>
       <c r="R31">
-        <v>-2.5</v>
-      </c>
-      <c r="S31">
-        <v>-3.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
       <c r="B32">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="C32">
         <v>4</v>
@@ -2411,49 +2324,46 @@
         <v>6.5</v>
       </c>
       <c r="F32">
+        <v>1000</v>
+      </c>
+      <c r="G32">
+        <v>1.5</v>
+      </c>
+      <c r="H32">
+        <v>7</v>
+      </c>
+      <c r="I32">
+        <v>7.5</v>
+      </c>
+      <c r="J32">
+        <v>-2.5</v>
+      </c>
+      <c r="K32">
+        <v>4</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>6</v>
+      </c>
+      <c r="N32">
+        <v>1.5</v>
+      </c>
+      <c r="O32">
+        <v>1.5</v>
+      </c>
+      <c r="P32">
         <v>4.5</v>
       </c>
-      <c r="G32">
+      <c r="Q32">
         <v>4</v>
       </c>
-      <c r="H32">
-        <v>4.5</v>
-      </c>
-      <c r="I32">
+      <c r="R32">
         <v>4</v>
       </c>
-      <c r="J32">
-        <v>4</v>
-      </c>
-      <c r="K32">
-        <v>6.5</v>
-      </c>
-      <c r="L32">
-        <v>4.5</v>
-      </c>
-      <c r="M32">
-        <v>4</v>
-      </c>
-      <c r="N32">
-        <v>4.5</v>
-      </c>
-      <c r="O32">
-        <v>4</v>
-      </c>
-      <c r="P32">
-        <v>4</v>
-      </c>
-      <c r="Q32">
-        <v>6.5</v>
-      </c>
-      <c r="R32">
-        <v>4.5</v>
-      </c>
-      <c r="S32">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -2470,46 +2380,43 @@
         <v>5.5</v>
       </c>
       <c r="F33">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="G33">
-        <v>6.5</v>
+        <v>1000</v>
       </c>
       <c r="H33">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="I33">
-        <v>6.5</v>
+        <v>3.5</v>
       </c>
       <c r="J33">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="K33">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="L33">
         <v>-1</v>
       </c>
       <c r="M33">
-        <v>6.5</v>
+        <v>3</v>
       </c>
       <c r="N33">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="O33">
-        <v>6.5</v>
+        <v>1</v>
       </c>
       <c r="P33">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q33">
-        <v>5.5</v>
+        <v>2</v>
       </c>
       <c r="R33">
-        <v>-1</v>
-      </c>
-      <c r="S33">
-        <v>6.5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>